<commit_message>
Working version (minus special classes)
</commit_message>
<xml_diff>
--- a/active_report.xlsx
+++ b/active_report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,9 +15,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="$#,###,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt formatCode="$#,###,##0.00" numFmtId="164"/>
+    <numFmt formatCode="#,##0.0" numFmtId="165"/>
+    <numFmt formatCode="0.0%" numFmtId="166"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -163,100 +163,100 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="17" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="18" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="21" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="22" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -620,34 +620,34 @@
   </sheetPr>
   <dimension ref="A1:V362"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0">
+    <sheetView colorId="64" defaultGridColor="1" showOutlineSymbols="1" showRuler="1" tabSelected="1" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="1" width="20" customWidth="1" min="1" max="1"/>
-    <col collapsed="1" width="12" customWidth="1" min="2" max="2"/>
-    <col collapsed="1" width="12" customWidth="1" min="3" max="3"/>
-    <col collapsed="1" width="18" customWidth="1" min="4" max="4"/>
-    <col collapsed="1" width="9" customWidth="1" min="5" max="5"/>
-    <col collapsed="1" width="20" customWidth="1" min="6" max="6"/>
-    <col collapsed="1" width="10" customWidth="1" min="7" max="7"/>
-    <col collapsed="1" width="9" customWidth="1" min="8" max="8"/>
-    <col collapsed="1" width="9" customWidth="1" min="9" max="9"/>
-    <col collapsed="1" width="9" customWidth="1" min="10" max="10"/>
-    <col collapsed="1" width="9" customWidth="1" min="11" max="11"/>
-    <col collapsed="1" width="13" customWidth="1" min="12" max="12"/>
-    <col collapsed="1" width="13" customWidth="1" min="13" max="13"/>
-    <col collapsed="1" width="13" customWidth="1" min="14" max="14"/>
-    <col collapsed="1" width="9" customWidth="1" min="15" max="15"/>
-    <col collapsed="1" width="8" customWidth="1" min="16" max="16"/>
-    <col collapsed="1" width="7" customWidth="1" min="17" max="17"/>
-    <col collapsed="1" width="7" customWidth="1" min="18" max="18"/>
-    <col collapsed="1" width="8" customWidth="1" min="19" max="19"/>
-    <col collapsed="1" width="6" customWidth="1" min="20" max="20"/>
-    <col collapsed="1" width="15" customWidth="1" min="21" max="21"/>
-    <col collapsed="1" width="17" customWidth="1" min="22" max="22"/>
+    <col collapsed="1" customWidth="1" max="1" min="1" width="20"/>
+    <col collapsed="1" customWidth="1" max="2" min="2" width="12"/>
+    <col collapsed="1" customWidth="1" max="3" min="3" width="12"/>
+    <col collapsed="1" customWidth="1" max="4" min="4" width="18"/>
+    <col collapsed="1" customWidth="1" max="5" min="5" width="9"/>
+    <col collapsed="1" customWidth="1" max="6" min="6" width="20"/>
+    <col collapsed="1" customWidth="1" max="7" min="7" width="10"/>
+    <col collapsed="1" customWidth="1" max="8" min="8" width="9"/>
+    <col collapsed="1" customWidth="1" max="9" min="9" width="9"/>
+    <col collapsed="1" customWidth="1" max="10" min="10" width="9"/>
+    <col collapsed="1" customWidth="1" max="11" min="11" width="9"/>
+    <col collapsed="1" customWidth="1" max="12" min="12" width="13"/>
+    <col collapsed="1" customWidth="1" max="13" min="13" width="13"/>
+    <col collapsed="1" customWidth="1" max="14" min="14" width="13"/>
+    <col collapsed="1" customWidth="1" max="15" min="15" width="9"/>
+    <col collapsed="1" customWidth="1" max="16" min="16" width="8"/>
+    <col collapsed="1" customWidth="1" max="17" min="17" width="7"/>
+    <col collapsed="1" customWidth="1" max="18" min="18" width="7"/>
+    <col collapsed="1" customWidth="1" max="19" min="19" width="8"/>
+    <col collapsed="1" customWidth="1" max="20" min="20" width="6"/>
+    <col collapsed="1" customWidth="1" max="21" min="21" width="15"/>
+    <col collapsed="1" customWidth="1" max="22" min="22" width="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -30365,6 +30365,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>